<commit_message>
optimized testcases by using baseapi.py
</commit_message>
<xml_diff>
--- a/testdatas/testcasedata.xlsx
+++ b/testdatas/testcasedata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9420" activeTab="3"/>
+    <workbookView windowWidth="21671" windowHeight="9840" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="框架使用说明" sheetId="6" r:id="rId1"/>
@@ -220,7 +220,7 @@
     <t>{"leave_amount":"$..leave_amount"}</t>
   </si>
   <si>
-    <t>[{"expression":"$..code","expected":0,"type":"equal"},{"expression":"$..msg","expected":"OK","type":"equal"},{"expression":"$..leave_amount","expected":#leave_amount#+1,"type":"equal"}]</t>
+    <t>[{"expression":"$..code","expected":0,"type":"equal"},{"expression":"$..msg","expected":"OK","type":"equal"},{"expression":"$..leave_amount","expected":round(#leave_amount#+1,2),"type":"equal"}]</t>
   </si>
   <si>
     <t>[{"sql":"select leave_amount from member where id='#member_id#'","expected":{'leave_amount':#leave_amount#+1},"type_db":"equal"}]</t>
@@ -232,7 +232,7 @@
     <t>{"member_id":#member_id#,"amount":2000}</t>
   </si>
   <si>
-    <t>[{"expression":"$..code","expected":0,"type":"equal"},{"expression":"$..msg","expected":"OK","type":"equal"},{"expression":"$..leave_amount","expected":#leave_amount#+2000,"type":"equal"}]</t>
+    <t>[{"expression":"$..code","expected":0,"type":"equal"},{"expression":"$..msg","expected":"OK","type":"equal"},{"expression":"$..leave_amount","expected":round(#leave_amount#+2000,2),"type":"equal"}]</t>
   </si>
   <si>
     <t>[{"sql":"select leave_amount from member where id='#member_id#'","expected":{'leave_amount':#leave_amount#+2000},"type_db":"equal"}]</t>
@@ -390,14 +390,90 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -419,84 +495,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -519,17 +519,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -542,13 +542,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -560,79 +698,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -644,85 +716,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -747,17 +747,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -773,6 +782,41 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -800,50 +844,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -852,10 +852,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="3">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="4">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0">
@@ -864,133 +864,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="4">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="7">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="16" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="18" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0">
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="32" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1365,7 +1365,7 @@
   <sheetPr/>
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -1827,13 +1827,13 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="6"/>
   <cols>
     <col min="1" max="1" width="4.44444444444444" customWidth="1"/>
-    <col min="2" max="2" width="15.1111111111111" customWidth="1"/>
+    <col min="2" max="2" width="22.4444444444444" customWidth="1"/>
     <col min="3" max="3" width="10.1111111111111" customWidth="1"/>
     <col min="5" max="5" width="17.3333333333333" customWidth="1"/>
     <col min="6" max="6" width="51.4444444444444" customWidth="1"/>
@@ -1894,7 +1894,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" ht="144" spans="1:9">
+    <row r="3" ht="158.4" spans="1:9">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1923,7 +1923,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" ht="144" spans="1:9">
+    <row r="4" ht="158.4" spans="1:9">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2039,7 +2039,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2"/>

</xml_diff>